<commit_message>
updated power breakdown with x48 and CPU power, need to double check CPU
</commit_message>
<xml_diff>
--- a/Excel Sheet/Power Breakdown.xlsx
+++ b/Excel Sheet/Power Breakdown.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="480" yWindow="75" windowWidth="14175" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Individual" sheetId="1" r:id="rId1"/>
+    <sheet name="Totals" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Power Requirements</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve"> 1.1 V/1.2 V</t>
   </si>
   <si>
-    <t xml:space="preserve"> Processor System Bus Power</t>
-  </si>
-  <si>
     <t>VCC_EXP</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>VCC_DDR</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1.5V1</t>
-  </si>
-  <si>
     <t xml:space="preserve"> DDR3 System Memory Power</t>
   </si>
   <si>
@@ -87,21 +81,12 @@
     <t xml:space="preserve"> Secondary PCI Express PLL Analog Power</t>
   </si>
   <si>
-    <t>VCCA_hplL</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Host PLL Analog Power</t>
   </si>
   <si>
-    <t>VCCA_mpl</t>
-  </si>
-  <si>
     <t xml:space="preserve"> System Memory PLL Analog Power</t>
   </si>
   <si>
-    <t>VCCABG_EXP</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 3.3 V</t>
   </si>
   <si>
@@ -130,6 +115,90 @@
   </si>
   <si>
     <t>1.25 V</t>
+  </si>
+  <si>
+    <t>VTT_FSB</t>
+  </si>
+  <si>
+    <t>VCCA_HPLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.5V</t>
+  </si>
+  <si>
+    <t>VCCA_MPLL</t>
+  </si>
+  <si>
+    <t>MCH Core</t>
+  </si>
+  <si>
+    <t>Host Interface</t>
+  </si>
+  <si>
+    <t>System Memory Interface</t>
+  </si>
+  <si>
+    <t>PCI Express</t>
+  </si>
+  <si>
+    <t>VCCA_EXP</t>
+  </si>
+  <si>
+    <t>CMOS Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Processor System Bus Power (Actual voltage varies by CPU)</t>
+  </si>
+  <si>
+    <t>Current (A)</t>
+  </si>
+  <si>
+    <t>1.1/1.2V</t>
+  </si>
+  <si>
+    <t>1.5V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
+  </si>
+  <si>
+    <t>X48</t>
+  </si>
+  <si>
+    <t>Total Current (A) by Voltage Rail</t>
+  </si>
+  <si>
+    <t>Core2 Duo 7500 CPU</t>
+  </si>
+  <si>
+    <t>VCC_BOOT</t>
+  </si>
+  <si>
+    <t>VCC_PLL</t>
+  </si>
+  <si>
+    <t>VTT_OUT_LEFT</t>
+  </si>
+  <si>
+    <t>VTT_OUT_RIGHT</t>
+  </si>
+  <si>
+    <t>VCC_GTLREF</t>
+  </si>
+  <si>
+    <t>1.1V</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>1.25V VCC</t>
+  </si>
+  <si>
+    <t>1.25V VTT</t>
+  </si>
+  <si>
+    <t>CPU</t>
   </si>
 </sst>
 </file>
@@ -182,13 +251,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,187 +557,336 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A2:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12">
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="21">
-      <c r="A4" s="2" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="4" spans="1:12" ht="21">
+      <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="J4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
+      <c r="I5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" s="6">
+        <v>8.99</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8">
+        <v>1.25</v>
+      </c>
+      <c r="K8">
+        <v>0.13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1.61</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>16</v>
+      <c r="J9">
+        <v>1.25</v>
+      </c>
+      <c r="K9">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="6">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10">
+        <v>1.25</v>
+      </c>
+      <c r="K10">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11">
+        <v>1.25</v>
+      </c>
+      <c r="K11">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" t="s">
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
+      <c r="I12" t="s">
+        <v>55</v>
+      </c>
+      <c r="J12">
+        <v>1.25</v>
+      </c>
+      <c r="K12">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C14" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" t="s">
+      <c r="D14" s="6">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="B13" t="s">
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D15" s="6">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" t="s">
+    <row r="16" spans="1:12">
+      <c r="A16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
         <v>23</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="D16" s="6">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" t="s">
+    <row r="17" spans="2:5">
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="5"/>
+      <c r="E17" t="s">
         <v>25</v>
       </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" t="s">
+      <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D18" s="5"/>
+      <c r="E18" t="s">
         <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="C2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -672,12 +895,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="C5">
+        <v>9.9990000000000006</v>
+      </c>
+      <c r="D5">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="E5">
+        <v>1.9770000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <v>75.150000000000006</v>
+      </c>
+      <c r="D6">
+        <v>5.76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>